<commit_message>
updated map and added Collector command
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Part Name</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t xml:space="preserve">port cam0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ball Collector Motor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Needs to be a talon hooked up to port 5 on the rio</t>
   </si>
 </sst>
 </file>
@@ -146,17 +152,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.5357142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -211,6 +218,17 @@
       </c>
       <c r="C6" s="0" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>